<commit_message>
add pagi siang 15
</commit_message>
<xml_diff>
--- a/SetelahRevisi/15-10-2019.xlsx
+++ b/SetelahRevisi/15-10-2019.xlsx
@@ -64,7 +64,7 @@
     <t xml:space="preserve">06:50 – 06:55</t>
   </si>
   <si>
-    <t xml:space="preserve">06:55 – 8:00</t>
+    <t xml:space="preserve">06:55 – 7:00</t>
   </si>
   <si>
     <t xml:space="preserve">11:00 – 11:05</t>
@@ -274,7 +274,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -292,6 +292,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -378,11 +382,11 @@
   </sheetPr>
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.95"/>
@@ -405,10 +409,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="n">
-        <v>185</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -416,10 +420,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="n">
-        <v>133</v>
+        <v>27</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -427,10 +431,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="n">
-        <v>131</v>
+        <v>33</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -438,10 +442,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="4" t="n">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -449,10 +453,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="4" t="n">
-        <v>122</v>
+        <v>46</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,233 +464,389 @@
         <v>8</v>
       </c>
       <c r="B7" s="4" t="n">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B8" s="5" t="n">
+        <v>43</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="B9" s="5" t="n">
+        <v>57</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="B10" s="5" t="n">
+        <v>134</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="B11" s="5" t="n">
+        <v>90</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B12" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="B13" s="5" t="n">
+        <v>130</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="B14" s="5" t="n">
+        <v>95</v>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="B15" s="5" t="n">
+        <v>132</v>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="B16" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="B17" s="5" t="n">
+        <v>123</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B18" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="C18" s="5" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B19" s="5" t="n">
+        <v>72</v>
+      </c>
+      <c r="C19" s="5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="B20" s="5" t="n">
+        <v>111</v>
+      </c>
+      <c r="C20" s="5" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="B21" s="5" t="n">
+        <v>143</v>
+      </c>
+      <c r="C21" s="5" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="B22" s="5" t="n">
+        <v>102</v>
+      </c>
+      <c r="C22" s="5" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="B23" s="5" t="n">
+        <v>95</v>
+      </c>
+      <c r="C23" s="5" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="B24" s="5" t="n">
+        <v>169</v>
+      </c>
+      <c r="C24" s="5" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B25" s="5" t="n">
+        <v>154</v>
+      </c>
+      <c r="C25" s="5" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
         <v>43</v>
       </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
         <v>45</v>
       </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
         <v>46</v>
       </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="0" t="n">
+      <c r="B50" s="5" t="n">
         <f aca="false">SUM(B2:B49)</f>
-        <v>782</v>
-      </c>
-      <c r="C50" s="0" t="n">
+        <v>2070</v>
+      </c>
+      <c r="C50" s="5" t="n">
         <f aca="false">SUM(C2:C49)</f>
-        <v>40</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>